<commit_message>
add: updated reports and runtime snapshots after FeatureEngine v1.1 validation
</commit_message>
<xml_diff>
--- a/reports/2026-01-18.xlsx
+++ b/reports/2026-01-18.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-18 06:29 UTC</t>
+          <t>2026-01-18 13:58 UTC</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -630,43 +630,43 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CAKEUSDT</t>
+          <t>EGLDUSDT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PancakeSwap</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$2.10</t>
+          <t>$6.55</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$722.54M</t>
+          <t>$191.42M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$1.74M</t>
+          <t>$2.09M</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>77.5</v>
+        <v>76.95</v>
       </c>
       <c r="H2" t="n">
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J2" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>59.73</v>
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
@@ -676,43 +676,43 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>GALAUSDT</t>
+          <t>MEUSDT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Gala</t>
+          <t>Magic Eden</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$0.01</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$360.21M</t>
+          <t>$124.94M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$3.18M</t>
+          <t>$4.03M</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>72.5</v>
+        <v>75</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" t="inlineStr"/>
     </row>
@@ -722,43 +722,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EGLDUSDT</t>
+          <t>MANAUSDT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MultiversX</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$6.75</t>
+          <t>$0.16</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$195.92M</t>
+          <t>$312.37M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$2.04M</t>
+          <t>$3.41M</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>71.2</v>
+        <v>75</v>
       </c>
       <c r="H4" t="n">
         <v>100</v>
       </c>
       <c r="I4" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>31.01</v>
+        <v>100</v>
       </c>
       <c r="L4" t="inlineStr"/>
     </row>
@@ -768,43 +768,43 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MANAUSDT</t>
+          <t>GALAUSDT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>Gala</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$0.16</t>
+          <t>$0.01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>$315.61M</t>
+          <t>$355.54M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$3.50M</t>
+          <t>$2.74M</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>67.43000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="H5" t="n">
         <v>100</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J5" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K5" t="n">
-        <v>62.15</v>
+        <v>0</v>
       </c>
       <c r="L5" t="inlineStr"/>
     </row>
@@ -814,43 +814,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CRVUSDT</t>
+          <t>SANDUSDT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Curve DAO Token</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$0.42</t>
+          <t>$0.15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>$605.45M</t>
+          <t>$389.86M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$1.61M</t>
+          <t>$4.68M</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>65.44</v>
+        <v>70.44</v>
       </c>
       <c r="H6" t="n">
-        <v>84.79000000000001</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>77.20999999999999</v>
       </c>
       <c r="L6" t="inlineStr"/>
     </row>
@@ -860,40 +860,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FILUSDT</t>
+          <t>CAKEUSDT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>PancakeSwap</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$1.53</t>
+          <t>$2.08</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$1.13B</t>
+          <t>$714.90M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$4.79M</t>
+          <t>$1.62M</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>65</v>
+        <v>67.5</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J7" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -906,43 +906,43 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IMXUSDT</t>
+          <t>BERAUSDT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Immutable</t>
+          <t>Berachain</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$0.29</t>
+          <t>$0.87</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$573.74M</t>
+          <t>$125.92M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$1.54M</t>
+          <t>$6.28M</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>65</v>
+        <v>65.76000000000001</v>
       </c>
       <c r="H8" t="n">
         <v>100</v>
       </c>
       <c r="I8" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>53.79</v>
       </c>
       <c r="L8" t="inlineStr"/>
     </row>
@@ -952,27 +952,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BONKUSDT</t>
+          <t>FILUSDT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bonk</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1.53</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$911.24M</t>
+          <t>$1.13B</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$1.13M</t>
+          <t>$3.90M</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -998,31 +998,31 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ARBUSDT</t>
+          <t>IMXUSDT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Immutable</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>$0.21</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$1.25B</t>
+          <t>$572.67M</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$3.26M</t>
+          <t>$1.26M</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>57.5</v>
+        <v>65</v>
       </c>
       <c r="H10" t="n">
         <v>100</v>
@@ -1031,7 +1031,7 @@
         <v>80</v>
       </c>
       <c r="J10" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -1044,31 +1044,31 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PENGUUSDT</t>
+          <t>BONKUSDT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pudgy Penguins</t>
+          <t>Bonk</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$0.01</t>
+          <t>$0.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$737.50M</t>
+          <t>$910.13M</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$2.20M</t>
+          <t>$1.03M</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>57.5</v>
+        <v>65</v>
       </c>
       <c r="H11" t="n">
         <v>100</v>
@@ -1077,7 +1077,7 @@
         <v>80</v>
       </c>
       <c r="J11" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1187,43 +1187,43 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MANAUSDT</t>
+          <t>SANDUSDT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$0.16</t>
+          <t>$0.15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$315.61M</t>
+          <t>$389.86M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$3.50M</t>
+          <t>$4.68M</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>58.57</v>
+        <v>65</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>93.22</v>
+        <v>100</v>
       </c>
       <c r="J2" t="n">
         <v>100</v>
       </c>
       <c r="K2" t="n">
-        <v>70.66</v>
+        <v>100</v>
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
@@ -1233,37 +1233,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SANDUSDT</t>
+          <t>MEUSDT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Magic Eden</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$0.15</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$407.00M</t>
+          <t>$124.94M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$5.27M</t>
+          <t>$4.03M</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>39.63</v>
+        <v>65</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>15.43</v>
+        <v>100</v>
       </c>
       <c r="J3" t="n">
         <v>100</v>
@@ -1279,43 +1279,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>METUSDT</t>
+          <t>MANAUSDT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Meteora</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$0.32</t>
+          <t>$0.16</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$158.11M</t>
+          <t>$312.37M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$2.43M</t>
+          <t>$3.41M</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>37.74</v>
+        <v>59.69</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>9.130000000000001</v>
+        <v>100</v>
       </c>
       <c r="J4" t="n">
         <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>100</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="L4" t="inlineStr"/>
     </row>
@@ -1335,27 +1335,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$0.96</t>
+          <t>$0.87</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>$138.00M</t>
+          <t>$125.92M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$7.53M</t>
+          <t>$6.28M</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>35.92</v>
+        <v>59.2</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>3.07</v>
+        <v>80.68000000000001</v>
       </c>
       <c r="J5" t="n">
         <v>100</v>
@@ -1371,43 +1371,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AXSUSDT</t>
+          <t>METUSDT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Axie Infinity</t>
+          <t>Meteora</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$2.04</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>$344.03M</t>
+          <t>$145.40M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$32.06M</t>
+          <t>$3.05M</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>35</v>
+        <v>57.23</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J6" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K6" t="n">
-        <v>100</v>
+        <v>61.5</v>
       </c>
       <c r="L6" t="inlineStr"/>
     </row>
@@ -1417,37 +1417,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DASHUSDT</t>
+          <t>AXSUSDT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dash</t>
+          <t>Axie Infinity</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$75.54</t>
+          <t>$1.87</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$946.27M</t>
+          <t>$318.20M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$30.21M</t>
+          <t>$26.86M</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>35</v>
+        <v>55.79</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>69.29000000000001</v>
       </c>
       <c r="J7" t="n">
         <v>100</v>
@@ -1463,43 +1463,43 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CHZUSDT</t>
+          <t>IPUSDT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Chiliz</t>
+          <t>Story</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$0.06</t>
+          <t>$2.67</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$637.22M</t>
+          <t>$936.31M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$26.87M</t>
+          <t>$5.15M</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>35</v>
+        <v>39.95</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>24.17</v>
       </c>
       <c r="J8" t="n">
         <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>100</v>
+        <v>84.68000000000001</v>
       </c>
       <c r="L8" t="inlineStr"/>
     </row>
@@ -1509,43 +1509,43 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ICPUSDT</t>
+          <t>EGLDUSDT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Internet Computer</t>
+          <t>MultiversX</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$4.01</t>
+          <t>$6.55</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$2.20B</t>
+          <t>$191.42M</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$8.85M</t>
+          <t>$2.09M</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>35</v>
+        <v>38.68</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="K9" t="n">
-        <v>100</v>
+        <v>25.37</v>
       </c>
       <c r="L9" t="inlineStr"/>
     </row>
@@ -1555,27 +1555,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ZENUSDT</t>
+          <t>DASHUSDT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Horizen</t>
+          <t>Dash</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>$11.64</t>
+          <t>$84.76</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$205.51M</t>
+          <t>$1.06B</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$6.00M</t>
+          <t>$28.01M</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1601,27 +1601,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IPUSDT</t>
+          <t>CHZUSDT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Story</t>
+          <t>Chiliz</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$2.83</t>
+          <t>$0.06</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$1.00B</t>
+          <t>$613.44M</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$4.55M</t>
+          <t>$21.44M</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1744,34 +1744,34 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BERAUSDT</t>
+          <t>MEUSDT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Berachain</t>
+          <t>Magic Eden</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$0.96</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$138.00M</t>
+          <t>$124.94M</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$7.53M</t>
+          <t>$4.03M</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>64.61</v>
+        <v>77</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I2" t="n">
         <v>20</v>
@@ -1780,7 +1780,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="n">
-        <v>23.07</v>
+        <v>100</v>
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
@@ -1790,43 +1790,43 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AXSUSDT</t>
+          <t>METUSDT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Axie Infinity</t>
+          <t>Meteora</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$2.04</t>
+          <t>$0.29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$344.03M</t>
+          <t>$145.40M</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$32.06M</t>
+          <t>$3.05M</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>63.24</v>
+        <v>70.5</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="I3" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K3" t="n">
-        <v>16.18</v>
+        <v>100</v>
       </c>
       <c r="L3" t="inlineStr"/>
     </row>
@@ -1836,43 +1836,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>METUSDT</t>
+          <t>AXSUSDT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Meteora</t>
+          <t>Axie Infinity</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$0.32</t>
+          <t>$1.87</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$158.11M</t>
+          <t>$318.20M</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$2.43M</t>
+          <t>$26.86M</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>62.83</v>
+        <v>63.5</v>
       </c>
       <c r="H4" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I4" t="n">
         <v>20</v>
       </c>
       <c r="J4" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K4" t="n">
-        <v>29.13</v>
+        <v>80</v>
       </c>
       <c r="L4" t="inlineStr"/>
     </row>
@@ -1882,31 +1882,31 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MANAUSDT</t>
+          <t>SANDUSDT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Decentraland</t>
+          <t>The Sandbox</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$0.16</t>
+          <t>$0.15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>$315.61M</t>
+          <t>$389.86M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$3.50M</t>
+          <t>$4.68M</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>57.5</v>
+        <v>61.5</v>
       </c>
       <c r="H5" t="n">
         <v>80</v>
@@ -1918,7 +1918,7 @@
         <v>50</v>
       </c>
       <c r="K5" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L5" t="inlineStr"/>
     </row>
@@ -1928,43 +1928,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IPUSDT</t>
+          <t>BERAUSDT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Story</t>
+          <t>Berachain</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$2.83</t>
+          <t>$0.87</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>$1.00B</t>
+          <t>$125.92M</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$4.55M</t>
+          <t>$6.28M</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>57</v>
+        <v>57.5</v>
       </c>
       <c r="H6" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I6" t="n">
         <v>20</v>
       </c>
       <c r="J6" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L6" t="inlineStr"/>
     </row>
@@ -1974,43 +1974,43 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SANDUSDT</t>
+          <t>MANAUSDT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>The Sandbox</t>
+          <t>Decentraland</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$0.15</t>
+          <t>$0.16</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$407.00M</t>
+          <t>$312.37M</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$5.27M</t>
+          <t>$3.41M</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>51.59</v>
+        <v>56.5</v>
       </c>
       <c r="H7" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="I7" t="n">
         <v>20</v>
       </c>
       <c r="J7" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="K7" t="n">
-        <v>35.43</v>
+        <v>100</v>
       </c>
       <c r="L7" t="inlineStr"/>
     </row>
@@ -2020,40 +2020,40 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RONUSDT</t>
+          <t>DASHUSDT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ronin</t>
+          <t>Dash</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$0.17</t>
+          <t>$84.76</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$125.08M</t>
+          <t>$1.06B</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$1.01M</t>
+          <t>$28.01M</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>50.5</v>
+        <v>55</v>
       </c>
       <c r="H8" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I8" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" t="n">
         <v>80</v>
-      </c>
-      <c r="J8" t="n">
-        <v>50</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -2076,21 +2076,21 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$24.78</t>
+          <t>$26.43</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$484.70M</t>
+          <t>$521.38M</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$4.11M</t>
+          <t>$5.03M</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>47.82</v>
+        <v>55</v>
       </c>
       <c r="H9" t="n">
         <v>100</v>
@@ -2099,10 +2099,10 @@
         <v>20</v>
       </c>
       <c r="J9" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="K9" t="n">
-        <v>1.59</v>
+        <v>0</v>
       </c>
       <c r="L9" t="inlineStr"/>
     </row>
@@ -2112,40 +2112,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ZBCNUSDT</t>
+          <t>ACHUSDT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Zebec Network</t>
+          <t>Alchemy Pay</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$0.01</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$326.30M</t>
+          <t>$118.97M</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$1.47M</t>
+          <t>$1.20M</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H10" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I10" t="n">
         <v>20</v>
       </c>
       <c r="J10" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -2158,40 +2158,40 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PAXGUSDT</t>
+          <t>ZENUSDT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PAX Gold</t>
+          <t>Horizen</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$4614.54</t>
+          <t>$12.47</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$1.77B</t>
+          <t>$219.52M</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$2.08M</t>
+          <t>$5.80M</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>45.5</v>
+        <v>50</v>
       </c>
       <c r="H11" t="n">
+        <v>100</v>
+      </c>
+      <c r="I11" t="n">
+        <v>20</v>
+      </c>
+      <c r="J11" t="n">
         <v>60</v>
-      </c>
-      <c r="I11" t="n">
-        <v>100</v>
-      </c>
-      <c r="J11" t="n">
-        <v>10</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>

</xml_diff>